<commit_message>
Añadidos mensajes de error, cambio de titulo en el panel derecho (Consultas), ahora se muestran solo los primeros 20 resultados, cambio en los estilos de la tabla, añadido un icono para reiniciar la tabla y la barra de busqueda. Cambio a background color blanco
</commit_message>
<xml_diff>
--- a/b.xlsx
+++ b/b.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\repositorios random\ecuador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0541263E-B9E9-4BC6-903B-A2F364902D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48678E6-6F44-4B6E-8BC3-6681BCD08351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9799" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9805" uniqueCount="1242">
   <si>
     <r>
       <rPr>
@@ -12297,6 +12297,18 @@
   </si>
   <si>
     <t>Guayaquil</t>
+  </si>
+  <si>
+    <t>ba6eac</t>
+  </si>
+  <si>
+    <t>b3399d</t>
+  </si>
+  <si>
+    <t>e65151</t>
+  </si>
+  <si>
+    <t>e62a2a</t>
   </si>
 </sst>
 </file>
@@ -12306,7 +12318,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -12348,6 +12360,12 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="10">
@@ -12489,7 +12507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -12652,6 +12670,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12957,10 +12978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1399"/>
+  <dimension ref="A1:I1399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A674" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A692" sqref="A692"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75"/>
@@ -12971,7 +12992,7 @@
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="10.7" customHeight="1">
+    <row r="1" spans="1:9" ht="10.7" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>1236</v>
       </c>
@@ -12986,7 +13007,7 @@
       </c>
       <c r="G1" s="26"/>
     </row>
-    <row r="2" spans="1:7" ht="10.35" customHeight="1">
+    <row r="2" spans="1:9" ht="10.35" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13001,7 +13022,7 @@
       </c>
       <c r="G2" s="27"/>
     </row>
-    <row r="3" spans="1:7" ht="10.35" customHeight="1">
+    <row r="3" spans="1:9" ht="10.35" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13016,7 +13037,7 @@
       </c>
       <c r="G3" s="28"/>
     </row>
-    <row r="4" spans="1:7" ht="10.35" customHeight="1">
+    <row r="4" spans="1:9" ht="10.35" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13029,9 +13050,17 @@
       <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="38"/>
-    </row>
-    <row r="5" spans="1:7" ht="10.35" customHeight="1">
+      <c r="G4" s="38" t="s">
+        <v>1233</v>
+      </c>
+      <c r="H4" s="57" t="s">
+        <v>1240</v>
+      </c>
+      <c r="I4" s="57" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="10.35" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13044,9 +13073,17 @@
       <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="39"/>
-    </row>
-    <row r="6" spans="1:7" ht="10.35" customHeight="1">
+      <c r="G5" s="39" t="s">
+        <v>1232</v>
+      </c>
+      <c r="H5" s="57" t="s">
+        <v>1238</v>
+      </c>
+      <c r="I5" s="57" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="10.35" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13061,7 +13098,7 @@
       </c>
       <c r="G6" s="50"/>
     </row>
-    <row r="7" spans="1:7" ht="10.35" customHeight="1">
+    <row r="7" spans="1:9" ht="10.35" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13075,7 +13112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="10.35" customHeight="1">
+    <row r="8" spans="1:9" ht="10.35" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13089,7 +13126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="10.35" customHeight="1">
+    <row r="9" spans="1:9" ht="10.35" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13103,7 +13140,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="10.35" customHeight="1">
+    <row r="10" spans="1:9" ht="10.35" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13117,7 +13154,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="10.35" customHeight="1">
+    <row r="11" spans="1:9" ht="10.35" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13131,7 +13168,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="10.35" customHeight="1">
+    <row r="12" spans="1:9" ht="10.35" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13145,7 +13182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="10.35" customHeight="1">
+    <row r="13" spans="1:9" ht="10.35" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13159,7 +13196,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="10.35" customHeight="1">
+    <row r="14" spans="1:9" ht="10.35" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13173,7 +13210,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="10.35" customHeight="1">
+    <row r="15" spans="1:9" ht="10.35" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>1237</v>
       </c>
@@ -13187,7 +13224,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="10.35" customHeight="1">
+    <row r="16" spans="1:9" ht="10.35" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>1237</v>
       </c>

</xml_diff>